<commit_message>
this is the second version of test file 4
added a new column
</commit_message>
<xml_diff>
--- a/test file 4.xlsx
+++ b/test file 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/warren/Documents/GIT test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C1173DF-72FF-0743-9E3D-46E492F5B059}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BD8B92-4D0E-C544-8E9F-5C82256FC29A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="26520" windowHeight="16040" xr2:uid="{4B9AA83B-BDCA-4740-B485-276977B451E5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>test file 1</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>test 4</t>
+  </si>
+  <si>
+    <t>another change</t>
   </si>
 </sst>
 </file>
@@ -396,32 +399,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140881D9-EC46-B645-8743-8AB421077944}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>